<commit_message>
after(before) installation to mac os
phew(anything wrong? check
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yihua/Documents/GitHub/sequen_samp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20B9B94-90EE-2247-A1E9-E7340CBC3D9E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F132B751-85A9-4C45-A0BE-C02B2715CFFC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14640" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{2A7E2358-C8C9-1942-A999-76AF63424E80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>kk</t>
   </si>
@@ -72,6 +72,37 @@
   <si>
     <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
    7.00   14.00   19.50   21.97   25.00   72.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+     12      22      29      32      39      91</t>
+  </si>
+  <si>
+    <t>79/100</t>
+  </si>
+  <si>
+    <t>90/91</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+   9.00   15.00   20.00   22.17   26.00   55.00</t>
+  </si>
+  <si>
+    <t>97/100</t>
+  </si>
+  <si>
+    <t>96/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+   7.00   14.00   17.00   19.28   22.00   61.00 </t>
+  </si>
+  <si>
+    <t>90/100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+   8.00   12.00   15.00   16.54   20.00   36.00 </t>
   </si>
 </sst>
 </file>
@@ -467,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD8C36D-D580-7344-BA47-C3E793673C31}">
-  <dimension ref="A5:J24"/>
+  <dimension ref="A5:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +646,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>10</v>
@@ -663,7 +694,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="91" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>14</v>
@@ -672,9 +703,76 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="I18:J23"/>
     <mergeCell ref="A19:A20"/>
@@ -684,5 +782,6 @@
     <mergeCell ref="B24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
try correlated and top 5 dofferentiation
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yihua/Documents/GitHub/sequen_samp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F132B751-85A9-4C45-A0BE-C02B2715CFFC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B689599A-DAA5-9F4C-A540-C78B4AEF1343}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14640" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{2A7E2358-C8C9-1942-A999-76AF63424E80}"/>
+    <workbookView xWindow="7240" yWindow="460" windowWidth="32960" windowHeight="18920" xr2:uid="{2A7E2358-C8C9-1942-A999-76AF63424E80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>kk</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Results for binomial bandit</t>
-  </si>
-  <si>
-    <t>Pros: On aeverage FFB needs fewer samples to obtain at least 70% of the optimal bandit</t>
   </si>
   <si>
     <t>at least 70% being the optimal arm in the final iteration</t>
@@ -103,6 +100,48 @@
   <si>
     <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
    8.00   12.00   15.00   16.54   20.00   36.00 </t>
+  </si>
+  <si>
+    <t>Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+   6.00   12.00   15.00   16.39   19.00   49.00</t>
+  </si>
+  <si>
+    <t>910/1000</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>(0.6443884 0.6172192 0.6016559 0.5825437 0.5736236). (22   2  37  82  17 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7397591 0.6983675 0.6976299 0.6534694 0.6494925 (13 33 11 31 12)</t>
+  </si>
+  <si>
+    <t>0.8208992 0.7382919 0.7233833 0.659824. (2  12  42   4  62)</t>
+  </si>
+  <si>
+    <t>top 5 prob and arm</t>
+  </si>
+  <si>
+    <t>at least % being the optimal arm in the final iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+   6.00    9.00    9.00    9.60   10.75   13.00 </t>
+  </si>
+  <si>
+    <t>27/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6798228 0.6694615 0.6218070 0.6108186 0.5406304.   27 22 28 23 32  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min. 1st Qu.  Median    Mean 3rd Qu.    Max. 
+   7.00    9.00   10.50   11.03   12.00   25.00 </t>
+  </si>
+  <si>
+    <t>72/100</t>
   </si>
 </sst>
 </file>
@@ -132,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -158,32 +197,189 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,15 +694,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD8C36D-D580-7344-BA47-C3E793673C31}">
-  <dimension ref="A5:J28"/>
+  <dimension ref="A5:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:F28"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:6" x14ac:dyDescent="0.2">
@@ -619,167 +818,274 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="3" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
+      <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="H23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="15">
+        <v>22</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" t="s">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" t="s">
+      <c r="H25" s="20">
+        <v>13</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" t="s">
+      <c r="H26" s="21"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="H27" s="21"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="H28" s="21"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:10" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="24">
         <v>0.7</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" t="s">
-        <v>22</v>
-      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="21"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="19"/>
+    </row>
+    <row r="31" spans="1:10" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="15">
+        <v>2</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30">
+        <v>27</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="16">
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="H25:H30"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="B24:F24"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="A18:G18"/>
-    <mergeCell ref="I18:J23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>